<commit_message>
helpfile fix to import_metadata
</commit_message>
<xml_diff>
--- a/src/import_metadata/auto.xlsx
+++ b/src/import_metadata/auto.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbdaniels/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saori\Documents\Github\stata-fork\src\import_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="12804" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -327,7 +324,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -364,6 +361,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -635,12 +635,12 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +678,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -716,7 +716,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -754,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -976,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>74</v>
       </c>

</xml_diff>